<commit_message>
Changes till INT Form
</commit_message>
<xml_diff>
--- a/EvoTax.1099/wwwroot/Templates/Form1099INTTemplate.xlsx
+++ b/EvoTax.1099/wwwroot/Templates/Form1099INTTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\Code Repos\EvoTaxes\EvoTax.1099\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FDAF82-3429-4E6F-8837-6BEAE47958F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6490D2F5-E54E-4FB0-A82A-4197F2510C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="160">
   <si>
     <t>Rcp TIN</t>
   </si>
@@ -497,7 +497,10 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Is Corrected</t>
+    <t>Is Corrected Form of 1099</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1488,8 +1491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ2" sqref="AJ2:AJ13"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AJ5" sqref="AJ5:AJ13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1759,7 +1762,7 @@
         <v>37</v>
       </c>
       <c r="AJ3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">

</xml_diff>